<commit_message>
Pivot table: DateTime type with empty value (Issue #859 fix) (#860)
issue #859 : Pivot table: DateTime type with empty value
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/BlankPivotTableField/BlankPivotTableField.xlsx
+++ b/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/BlankPivotTableField/BlankPivotTableField.xlsx
@@ -11,14 +11,16 @@
     <x:sheet name="pvt2" sheetId="4" r:id="rId4"/>
     <x:sheet name="pvt3" sheetId="5" r:id="rId5"/>
     <x:sheet name="pvt4" sheetId="6" r:id="rId6"/>
+    <x:sheet name="pvt5" sheetId="7" r:id="rId7"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
   <x:pivotCaches>
-    <x:pivotCache cacheId="0" r:id="rId10"/>
-    <x:pivotCache cacheId="1" r:id="rId13"/>
-    <x:pivotCache cacheId="2" r:id="rId16"/>
-    <x:pivotCache cacheId="3" r:id="rId19"/>
+    <x:pivotCache cacheId="0" r:id="rId11"/>
+    <x:pivotCache cacheId="1" r:id="rId14"/>
+    <x:pivotCache cacheId="2" r:id="rId17"/>
+    <x:pivotCache cacheId="3" r:id="rId20"/>
+    <x:pivotCache cacheId="4" r:id="rId23"/>
   </x:pivotCaches>
 </x:workbook>
 </file>
@@ -117,13 +119,17 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -369,6 +375,127 @@
       <x:x/>
     </x:i>
     <x:i/>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:colItems>
+  <x:dataFields count="1">
+    <x:dataField name="NumberOfOrdersPercentageOfBearclaw" fld="2" subtotal="sum" showDataAs="percent" baseField="0" baseItem="2" numFmtId="165"/>
+  </x:dataFields>
+  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
+    </x:ext>
+  </x:extLst>
+</x:pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pvt5" cacheId="4" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
+  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <x:pivotFields count="6">
+    <x:pivotField name="Name" axis="axisCol" defaultSubtotal="0">
+      <x:items count="5">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Code" defaultSubtotal="0"/>
+    <x:pivotField name="NumberOfOrders" dataField="1" defaultSubtotal="0"/>
+    <x:pivotField name="Quality" defaultSubtotal="0"/>
+    <x:pivotField name="Month" defaultSubtotal="0"/>
+    <x:pivotField name="BakeDate" axis="axisRow" defaultSubtotal="0">
+      <x:items count="14">
+        <x:item x="0"/>
+        <x:item x="1"/>
+        <x:item x="2"/>
+        <x:item x="3"/>
+        <x:item x="4"/>
+        <x:item x="5"/>
+        <x:item x="6"/>
+        <x:item x="7"/>
+        <x:item x="8"/>
+        <x:item x="9"/>
+        <x:item x="10"/>
+        <x:item x="11"/>
+        <x:item x="12"/>
+        <x:item x="13"/>
+      </x:items>
+    </x:pivotField>
+  </x:pivotFields>
+  <x:rowFields count="1">
+    <x:field x="5"/>
+  </x:rowFields>
+  <x:rowItems count="15">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
+    <x:i>
+      <x:x v="5"/>
+    </x:i>
+    <x:i>
+      <x:x v="6"/>
+    </x:i>
+    <x:i>
+      <x:x v="7"/>
+    </x:i>
+    <x:i>
+      <x:x v="8"/>
+    </x:i>
+    <x:i>
+      <x:x v="9"/>
+    </x:i>
+    <x:i>
+      <x:x v="10"/>
+    </x:i>
+    <x:i>
+      <x:x v="11"/>
+    </x:i>
+    <x:i>
+      <x:x v="12"/>
+    </x:i>
+    <x:i>
+      <x:x v="13"/>
+    </x:i>
+    <x:i t="grand">
+      <x:x/>
+    </x:i>
+  </x:rowItems>
+  <x:colFields count="1">
+    <x:field x="0"/>
+  </x:colFields>
+  <x:colItems count="6">
+    <x:i>
+      <x:x v="0"/>
+    </x:i>
+    <x:i>
+      <x:x v="1"/>
+    </x:i>
+    <x:i>
+      <x:x v="2"/>
+    </x:i>
+    <x:i>
+      <x:x v="3"/>
+    </x:i>
+    <x:i>
+      <x:x v="4"/>
+    </x:i>
     <x:i t="grand">
       <x:x/>
     </x:i>
@@ -888,9 +1015,7 @@
       <x:c r="D11" s="0" t="n">
         <x:v>-20.24</x:v>
       </x:c>
-      <x:c r="F11" s="1">
-        <x:v>42849</x:v>
-      </x:c>
+      <x:c r="F11" s="2" t="s"/>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="A12" s="0" t="s">
@@ -994,7 +1119,7 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="1">
-    <x:tablePart r:id="rId9"/>
+    <x:tablePart r:id="rId10"/>
   </x:tableParts>
 </x:worksheet>
 </file>
@@ -1087,6 +1212,28 @@
 </x:worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
 <file path=pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
   <x:cacheSource type="worksheet">
@@ -1115,7 +1262,7 @@
       <x:sharedItems containsBlank="1"/>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="14"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1149,7 +1296,7 @@
       <x:sharedItems containsBlank="1"/>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="14"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1183,7 +1330,7 @@
       <x:sharedItems containsBlank="1"/>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="14"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
@@ -1217,12 +1364,62 @@
       <x:sharedItems containsBlank="1"/>
     </x:cacheField>
     <x:cacheField name="BakeDate">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="15"/>
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="14"/>
     </x:cacheField>
   </x:cacheFields>
 </x:pivotCacheDefinition>
 </file>
 
+<file path=pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" saveData="1" refreshOnLoad="1">
+  <x:cacheSource type="worksheet">
+    <x:worksheetSource name="PastrySalesData"/>
+  </x:cacheSource>
+  <x:cacheFields>
+    <x:cacheField name="Name">
+      <x:sharedItems count="5">
+        <x:s v="Croissant"/>
+        <x:s v="Doughnut"/>
+        <x:s v="Bearclaw"/>
+        <x:s v="Danish"/>
+        <x:s v="Scone"/>
+      </x:sharedItems>
+    </x:cacheField>
+    <x:cacheField name="Code">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="105" count="5"/>
+    </x:cacheField>
+    <x:cacheField name="NumberOfOrders">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="122" maxValue="394" count="14"/>
+    </x:cacheField>
+    <x:cacheField name="Quality">
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-20.24" maxValue="89.99" count="16"/>
+    </x:cacheField>
+    <x:cacheField name="Month">
+      <x:sharedItems containsBlank="1"/>
+    </x:cacheField>
+    <x:cacheField name="BakeDate">
+      <x:sharedItems containsSemiMixedTypes="1" containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-04-21T00:00:00" maxDate="2017-06-14T00:00:00" count="14">
+        <x:d v="2016-04-21T00:00:00"/>
+        <x:d v="2016-05-03T00:00:00"/>
+        <x:d v="2016-06-24T00:00:00"/>
+        <x:d v="2017-04-23T00:00:00"/>
+        <x:d v="2016-05-24T00:00:00"/>
+        <x:d v="2016-06-02T00:00:00"/>
+        <x:d v="2016-04-27T00:00:00"/>
+        <x:d v="2016-05-20T00:00:00"/>
+        <x:d v="2017-06-05T00:00:00"/>
+        <x:d v="2017-05-08T00:00:00"/>
+        <x:d v="2016-06-21T00:00:00"/>
+        <x:d v="2017-04-22T00:00:00"/>
+        <x:d v="2017-05-03T00:00:00"/>
+        <x:d v="2017-06-14T00:00:00"/>
+        <x:m/>
+      </x:sharedItems>
+    </x:cacheField>
+  </x:cacheFields>
+</x:pivotCacheDefinition>
+</file>
+
 <file path=pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1237,4 +1434,8 @@
 
 <file path=pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:pivotCacheRecords xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
</xml_diff>